<commit_message>
Roo is up and running
also changes `first` to `prefix` and `prefix_suffix` to `p_s`
</commit_message>
<xml_diff>
--- a/public/assets/data/atest.xlsx
+++ b/public/assets/data/atest.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>a</t>
   </si>
@@ -190,12 +190,45 @@
   </si>
   <si>
     <t>-ado</t>
+  </si>
+  <si>
+    <t>chico, -a</t>
+  </si>
+  <si>
+    <t>Adjective, Noun</t>
+  </si>
+  <si>
+    <t>small; (masc.) "boy," "child;" (fem.) "girl"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perhaps from Latin ciccus "nothing," earlier "something worthless," but originally "the thin membrane surrounding the grains of a pomegranate." Presumably borrowed from an unattested Ancient Greek word *κίκκος (kíkkos) "shell of a pomegranate," hypothesized by Beekes (2008) on the basis of the Latin word and possible Greek derivatives κίκκαβος (kíkkabos) "small coin in the Underworld," κικκάβι(ο)ν (kikkábi(o)n) "nothing," and κικαῖος (kikaios) of obscure meaning. </t>
+  </si>
+  <si>
+    <t>Ultimately of unknown origin.</t>
+  </si>
+  <si>
+    <t>The sense of "small" was first and then was extended to children. The change from c- to ch- in Spanish and Asturian is unexpected and may be due to Basque influence, via  txiki "small," "few," from earlier tiki. However, the change is not unique (e.g. Latin cicer "chick-pea" &gt; Spanish chícharo "pea").</t>
+  </si>
+  <si>
+    <t>llegar</t>
+  </si>
+  <si>
+    <t>to arrive</t>
+  </si>
+  <si>
+    <t>From Latin plicare "to fold." According to Roberts (2014), an extension of the sense of being 'folded' into something as an arrival at a destination.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From Proto-Italic *plek- 'id.' From Proto-Indo-European *pleḱ- 'id.' </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="\(@\)"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -244,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -269,6 +302,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,11 +609,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -585,7 +621,7 @@
     <col min="1" max="1" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="10" customWidth="1"/>
     <col min="5" max="5" width="15" style="2" customWidth="1"/>
     <col min="6" max="6" width="22.1640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="13.83203125" style="2" customWidth="1"/>
@@ -640,7 +676,7 @@
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -668,7 +704,6 @@
       <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
         <v>3</v>
       </c>
@@ -692,7 +727,6 @@
       <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
         <v>25</v>
       </c>
@@ -718,7 +752,6 @@
       <c r="C5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
         <v>40</v>
       </c>
@@ -740,7 +773,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="7" t="s">
@@ -764,7 +797,7 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="7" t="s">
@@ -788,7 +821,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="7" t="s">
@@ -812,7 +845,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="6"/>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="10" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -833,6 +866,43 @@
       </c>
       <c r="K9" s="7"/>
       <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A1:L979">

</xml_diff>

<commit_message>
Updates excel test file
</commit_message>
<xml_diff>
--- a/public/assets/data/atest.xlsx
+++ b/public/assets/data/atest.xlsx
@@ -612,8 +612,8 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>